<commit_message>
All functions for main script written and modulared into seperate files for structure and readability
</commit_message>
<xml_diff>
--- a/data/raw/comptages_terrain/activites_loisirs/us_med_pnmcca_observatoire_comptage_terrain_activites_loisirs_2021-07-28.xlsx
+++ b/data/raw/comptages_terrain/activites_loisirs/us_med_pnmcca_observatoire_comptage_terrain_activites_loisirs_2021-07-28.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12180" activeTab="2"/>
+    <workbookView windowWidth="18345" windowHeight="12180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_comptages" sheetId="28" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="37">
   <si>
     <t>Secteur</t>
   </si>
@@ -133,12 +133,10 @@
 1 peche - 2 pers</t>
   </si>
   <si>
-    <t>1 foil electrique</t>
-  </si>
-  <si>
     <t>Chasse sous-marine
 1 paddle - 1 pers
-2 jet - 1 pers</t>
+2 jet - 1 pers 
+Autre motonautique : foil eletrique</t>
   </si>
   <si>
     <t>1 kayak - 2 pers</t>
@@ -2041,8 +2039,8 @@
   <sheetPr/>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:Q2"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -2193,7 +2191,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="116" customHeight="1" spans="1:17">
+    <row r="4" s="1" customFormat="1" ht="296" customHeight="1" spans="1:17">
       <c r="A4" s="12">
         <v>0.5</v>
       </c>
@@ -2224,8 +2222,8 @@
       <c r="J4" s="13">
         <v>0</v>
       </c>
-      <c r="K4" s="13" t="s">
-        <v>33</v>
+      <c r="K4" s="13">
+        <v>1</v>
       </c>
       <c r="L4" s="13">
         <v>0</v>
@@ -2243,7 +2241,7 @@
         <v>5</v>
       </c>
       <c r="Q4" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="116" customHeight="1" spans="1:17">
@@ -2660,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="69.75" customHeight="1" spans="1:17">
@@ -2766,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="2:2">
@@ -3020,7 +3018,7 @@
         <v>5</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="69.75" customHeight="1" spans="1:17">
@@ -3073,7 +3071,7 @@
         <v>5</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="69.75" customHeight="1" spans="1:17">

</xml_diff>